<commit_message>
Implemented Safety routine, Flight Mode routine, Master Flight Controller routine and several other tweaks. Also modified the calibration method for BMP388.
</commit_message>
<xml_diff>
--- a/Docs/Drone Project - Software Stack Implementation.xlsx
+++ b/Docs/Drone Project - Software Stack Implementation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Standard Account\Desktop\College\6th sem\System Integration\Project\Code versions\DroneProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Standard Account\Desktop\College\6th sem\System Integration\Project\Code versions\DroneProject\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A6715F-6020-486D-A6E7-68FDC91E448E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCF0A20-E6EF-4CC0-93F0-1EEA27CD097D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FD653329-EDCD-44B8-92A5-0A478F126116}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -531,12 +531,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -544,9 +544,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -868,8 +865,8 @@
   </sheetPr>
   <dimension ref="B1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:R43"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -913,21 +910,21 @@
       <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="25">
         <v>44636</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="4"/>
@@ -991,7 +988,7 @@
       <c r="O8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="25"/>
+      <c r="Q8" s="24"/>
       <c r="R8" s="1" t="s">
         <v>48</v>
       </c>
@@ -1044,7 +1041,7 @@
         <v>47</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="4"/>

</xml_diff>

<commit_message>
Updated software stack diagram.
</commit_message>
<xml_diff>
--- a/Docs/Drone Project - Software Stack Implementation.xlsx
+++ b/Docs/Drone Project - Software Stack Implementation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Standard Account\Desktop\College\6th sem\System Integration\Project\Code versions\DroneProject\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\6th sem\23  mar\DroneProject\DroneProject\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCF0A20-E6EF-4CC0-93F0-1EEA27CD097D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9DCD0E-F916-403E-88EE-CAA4EBA63D11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FD653329-EDCD-44B8-92A5-0A478F126116}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD653329-EDCD-44B8-92A5-0A478F126116}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -178,9 +177,6 @@
     <t>Currently working on it</t>
   </si>
   <si>
-    <t>Kalman Filter (sensor fusion)</t>
-  </si>
-  <si>
     <t>To be done next</t>
   </si>
   <si>
@@ -200,6 +196,9 @@
   </si>
   <si>
     <t>Date:</t>
+  </si>
+  <si>
+    <t>Complimantary Filter (sensor fusion)</t>
   </si>
 </sst>
 </file>
@@ -528,9 +527,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -544,6 +540,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -866,56 +865,56 @@
   <dimension ref="B1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="28.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1"/>
+    <col min="9" max="9" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="1"/>
     <col min="13" max="13" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1"/>
-    <col min="15" max="15" width="22.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.88671875" style="1"/>
-    <col min="18" max="18" width="32.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="8.85546875" style="1"/>
+    <col min="15" max="15" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.85546875" style="1"/>
+    <col min="18" max="18" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="3" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="25">
-        <v>44636</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="24">
+        <v>44643</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="13" t="s">
         <v>0</v>
       </c>
@@ -944,7 +943,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -963,19 +962,19 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G7" s="12"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="26" t="s">
+    <row r="8" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="27"/>
       <c r="F8" s="17"/>
       <c r="G8" s="2"/>
       <c r="H8" s="4"/>
@@ -988,18 +987,18 @@
       <c r="O8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="24"/>
+      <c r="Q8" s="23"/>
       <c r="R8" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15"/>
       <c r="C9" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="11"/>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="28" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="18"/>
@@ -1014,7 +1013,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="7"/>
     </row>
-    <row r="10" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -1029,16 +1028,16 @@
       <c r="N10" s="9"/>
       <c r="O10" s="10"/>
     </row>
-    <row r="11" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O11" s="12"/>
     </row>
-    <row r="12" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="19" t="s">
-        <v>47</v>
+      <c r="E12" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="13" t="s">
@@ -1055,7 +1054,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -1070,10 +1069,10 @@
       <c r="N13" s="9"/>
       <c r="O13" s="10"/>
     </row>
-    <row r="14" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O14" s="12"/>
     </row>
-    <row r="15" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="13" t="s">
         <v>13</v>
       </c>
@@ -1097,10 +1096,10 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -1115,10 +1114,10 @@
       <c r="N16" s="9"/>
       <c r="O16" s="10"/>
     </row>
-    <row r="17" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O17" s="12"/>
     </row>
-    <row r="18" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="13" t="s">
         <v>18</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -1160,8 +1159,8 @@
       <c r="N19" s="9"/>
       <c r="O19" s="10"/>
     </row>
-    <row r="20" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="13" t="s">
         <v>23</v>
       </c>
@@ -1180,7 +1179,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="6"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1195,7 +1194,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="13" t="s">
         <v>24</v>
       </c>
@@ -1222,7 +1221,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="6"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1239,7 +1238,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1254,12 +1253,12 @@
       <c r="N25" s="9"/>
       <c r="O25" s="10"/>
     </row>
-    <row r="26" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O26" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -1277,10 +1276,10 @@
       <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
     </row>
-    <row r="28" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="2"/>
     </row>
-    <row r="30" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1297,7 +1296,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1312,7 +1311,7 @@
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1327,7 +1326,7 @@
       <c r="N32" s="4"/>
       <c r="O32" s="5"/>
     </row>
-    <row r="33" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="6"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1342,7 +1341,7 @@
       <c r="N33" s="2"/>
       <c r="O33" s="7"/>
     </row>
-    <row r="34" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="6"/>
       <c r="D34" s="2"/>
       <c r="E34" s="14" t="s">
@@ -1367,7 +1366,7 @@
       <c r="N34" s="2"/>
       <c r="O34" s="7"/>
     </row>
-    <row r="35" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="6"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1386,7 +1385,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="6"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1409,7 +1408,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="6"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1424,7 +1423,7 @@
       <c r="N37" s="2"/>
       <c r="O37" s="7"/>
     </row>
-    <row r="38" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="6"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1443,13 +1442,13 @@
       <c r="N38" s="2"/>
       <c r="O38" s="7"/>
     </row>
-    <row r="39" spans="3:18" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:18" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C39" s="6"/>
       <c r="D39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="7"/>
     </row>
-    <row r="40" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="6"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1464,7 +1463,7 @@
       <c r="N40" s="2"/>
       <c r="O40" s="7"/>
     </row>
-    <row r="41" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>

</xml_diff>

<commit_message>
Implemented and tested bluetooth module. Added Tuning interface support for various P+I controllers via Bluetooth module.
</commit_message>
<xml_diff>
--- a/Docs/Drone Project - Software Stack Implementation.xlsx
+++ b/Docs/Drone Project - Software Stack Implementation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\6th sem\23  mar\DroneProject\DroneProject\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Standard Account\Desktop\College\6th sem\System Integration\Project\Code versions\DroneProject\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9DCD0E-F916-403E-88EE-CAA4EBA63D11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA619D7-3B4B-486B-A409-68B1657C17ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD653329-EDCD-44B8-92A5-0A478F126116}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FD653329-EDCD-44B8-92A5-0A478F126116}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>Safety routine</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Altitude P-Controller</t>
   </si>
   <si>
-    <t>Roll, Pitch, Yaw PID Controllers</t>
-  </si>
-  <si>
     <t>Manual Controller</t>
   </si>
   <si>
@@ -199,6 +196,18 @@
   </si>
   <si>
     <t>Complimantary Filter (sensor fusion)</t>
+  </si>
+  <si>
+    <t>BLUETOOTH STDIO</t>
+  </si>
+  <si>
+    <t>Controller Tuning Interface</t>
+  </si>
+  <si>
+    <t>BLUETOOTH</t>
+  </si>
+  <si>
+    <t>Roll, Pitch, Yaw, Height PID Controllers</t>
   </si>
 </sst>
 </file>
@@ -533,6 +542,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -540,9 +552,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -864,57 +873,57 @@
   </sheetPr>
   <dimension ref="B1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="1"/>
-    <col min="5" max="5" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="1"/>
-    <col min="9" max="9" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="1"/>
-    <col min="13" max="13" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="1"/>
-    <col min="15" max="15" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.85546875" style="1"/>
-    <col min="18" max="18" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="35.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="1"/>
+    <col min="15" max="15" width="22.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.88671875" style="1"/>
+    <col min="18" max="18" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="3" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E3" s="24">
         <v>44643</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="13" t="s">
         <v>0</v>
       </c>
@@ -931,19 +940,21 @@
         <v>3</v>
       </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="K5" s="13" t="s">
+        <v>55</v>
+      </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q5" s="21"/>
       <c r="R5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -959,22 +970,22 @@
       <c r="O6" s="10"/>
       <c r="Q6" s="22"/>
       <c r="R6" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G7" s="12"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="17"/>
       <c r="G8" s="2"/>
       <c r="H8" s="4"/>
@@ -985,26 +996,26 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q8" s="23"/>
       <c r="R8" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="15"/>
       <c r="C9" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="11"/>
-      <c r="E9" s="28" t="s">
-        <v>6</v>
+      <c r="E9" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="F9" s="18"/>
       <c r="H9" s="2"/>
       <c r="I9" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1013,7 +1024,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="7"/>
     </row>
-    <row r="10" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -1028,20 +1039,20 @@
       <c r="N10" s="9"/>
       <c r="O10" s="10"/>
     </row>
-    <row r="11" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O11" s="12"/>
     </row>
-    <row r="12" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1051,10 +1062,10 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -1069,37 +1080,39 @@
       <c r="N13" s="9"/>
       <c r="O13" s="10"/>
     </row>
-    <row r="14" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O14" s="12"/>
     </row>
-    <row r="15" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="M15" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -1114,37 +1127,37 @@
       <c r="N16" s="9"/>
       <c r="O16" s="10"/>
     </row>
-    <row r="17" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O17" s="12"/>
     </row>
-    <row r="18" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -1159,13 +1172,15 @@
       <c r="N19" s="9"/>
       <c r="O19" s="10"/>
     </row>
-    <row r="20" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1176,10 +1191,10 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="6"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1194,34 +1209,34 @@
       <c r="N22" s="2"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C23" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C24" s="6"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1231,14 +1246,14 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1253,12 +1268,12 @@
       <c r="N25" s="9"/>
       <c r="O25" s="10"/>
     </row>
-    <row r="26" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O26" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -1276,10 +1291,10 @@
       <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
     </row>
-    <row r="28" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E28" s="2"/>
     </row>
-    <row r="30" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1293,10 +1308,10 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1311,7 +1326,7 @@
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="3"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1326,7 +1341,7 @@
       <c r="N32" s="4"/>
       <c r="O32" s="5"/>
     </row>
-    <row r="33" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="6"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1341,32 +1356,32 @@
       <c r="N33" s="2"/>
       <c r="O33" s="7"/>
     </row>
-    <row r="34" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C34" s="6"/>
       <c r="D34" s="2"/>
       <c r="E34" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="7"/>
     </row>
-    <row r="35" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C35" s="6"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1382,33 +1397,35 @@
       <c r="O35" s="7"/>
       <c r="Q35" s="20"/>
       <c r="R35" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C36" s="6"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
+      <c r="I36" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="J36" s="2"/>
       <c r="K36" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="7"/>
       <c r="Q36" s="21"/>
       <c r="R36" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C37" s="6"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1423,7 +1440,7 @@
       <c r="N37" s="2"/>
       <c r="O37" s="7"/>
     </row>
-    <row r="38" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C38" s="6"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1433,22 +1450,22 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L38" s="2"/>
       <c r="M38" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="7"/>
     </row>
-    <row r="39" spans="3:18" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:18" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C39" s="6"/>
       <c r="D39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="7"/>
     </row>
-    <row r="40" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="6"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1463,7 +1480,7 @@
       <c r="N40" s="2"/>
       <c r="O40" s="7"/>
     </row>
-    <row r="41" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>

</xml_diff>

<commit_message>
Final Submission. This is not the perfect flight controller, but it works fine.
</commit_message>
<xml_diff>
--- a/Docs/Drone Project - Software Stack Implementation.xlsx
+++ b/Docs/Drone Project - Software Stack Implementation.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Standard Account\Desktop\College\6th sem\System Integration\Project\Code versions\DroneProject\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Standard Account\Desktop\College\6th sem\System Integration\Project\Code versions\From College\DroneProject\DroneProject\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA619D7-3B4B-486B-A409-68B1657C17ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6F62E4-34B2-4A2D-99F6-13AF41100E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FD653329-EDCD-44B8-92A5-0A478F126116}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FD653329-EDCD-44B8-92A5-0A478F126116}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
   <si>
     <t>Safety routine</t>
   </si>
@@ -223,7 +224,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +255,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -468,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -545,6 +552,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -552,6 +598,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -873,8 +928,8 @@
   </sheetPr>
   <dimension ref="B1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -981,11 +1036,11 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="17"/>
       <c r="G8" s="2"/>
       <c r="H8" s="4"/>
@@ -1502,4 +1557,643 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="39" fitToWidth="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E71F8A-710A-40A2-8D70-308A98741E7B}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:R41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="35.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="1"/>
+    <col min="15" max="15" width="22.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.88671875" style="1"/>
+    <col min="18" max="18" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="24">
+        <v>44643</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="27"/>
+      <c r="K5" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="34"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="12"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="15"/>
+      <c r="C9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="38"/>
+      <c r="E9" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="36"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="31"/>
+    </row>
+    <row r="10" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="32"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="34"/>
+    </row>
+    <row r="11" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O11" s="12"/>
+    </row>
+    <row r="12" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="32"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="34"/>
+    </row>
+    <row r="14" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O14" s="12"/>
+    </row>
+    <row r="15" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="27"/>
+      <c r="G15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="27"/>
+      <c r="I15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="27"/>
+      <c r="K15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="27"/>
+      <c r="M15" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="N15" s="27"/>
+      <c r="O15" s="28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="32"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="34"/>
+    </row>
+    <row r="17" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O17" s="12"/>
+    </row>
+    <row r="18" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="27"/>
+      <c r="G18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="27"/>
+      <c r="I18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="27"/>
+      <c r="K18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="34"/>
+    </row>
+    <row r="20" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="31"/>
+    </row>
+    <row r="23" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="30"/>
+      <c r="E23" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="30"/>
+      <c r="G23" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="30"/>
+      <c r="I23" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" s="30"/>
+      <c r="K23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="30"/>
+      <c r="M23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="N23" s="30"/>
+      <c r="O23" s="31"/>
+    </row>
+    <row r="24" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="31"/>
+    </row>
+    <row r="25" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="32"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="34"/>
+    </row>
+    <row r="26" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+    </row>
+    <row r="28" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="30" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="5"/>
+    </row>
+    <row r="33" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="6"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="7"/>
+    </row>
+    <row r="34" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="6"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J34" s="2"/>
+      <c r="K34" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="L34" s="2"/>
+      <c r="M34" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="N34" s="2"/>
+      <c r="O34" s="7"/>
+    </row>
+    <row r="35" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="6"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="7"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="6"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J36" s="2"/>
+      <c r="K36" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L36" s="2"/>
+      <c r="M36" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N36" s="2"/>
+      <c r="O36" s="7"/>
+      <c r="Q36" s="21"/>
+      <c r="R36" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="6"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" spans="3:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="6"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="L38" s="2"/>
+      <c r="M38" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="N38" s="2"/>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" spans="3:18" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="6"/>
+      <c r="D39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="7"/>
+    </row>
+    <row r="40" spans="3:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="6"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="7"/>
+    </row>
+    <row r="41" spans="3:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="59" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>